<commit_message>
Subjects File Addition in Process
Subjects File Addition in Process
</commit_message>
<xml_diff>
--- a/Batch 2018-20/Sem 1/Grade Card.xlsx
+++ b/Batch 2018-20/Sem 1/Grade Card.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\AutoMBA\Results Genetaor\Batch 2018-20\Sem 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Git\SIMSR-Results-Generator\Batch 2018-20\Sem 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA58EF5-C240-4AFD-B600-0F160BAC8C06}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431D2EB4-7E0E-4344-B319-0A34D11B6878}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4C80AD8E-6BB5-43FA-A2DF-2A6A1A9D1C00}"/>
   </bookViews>
@@ -18,6 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="PicUp">INDEX([1]Sheet1!$C$2:$C$121,MATCH('Final Grade Card'!$D$13:$O$13,[1]Sheet1!$A$2:$A$121,0))</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>University of Mumbai</t>
   </si>
@@ -66,30 +67,6 @@
   </si>
   <si>
     <t>Total Marks</t>
-  </si>
-  <si>
-    <t>Perspective Management</t>
-  </si>
-  <si>
-    <t>Financial Accounting</t>
-  </si>
-  <si>
-    <t>Business Statistics</t>
-  </si>
-  <si>
-    <t>Operations Management</t>
-  </si>
-  <si>
-    <t>Managerial Economics</t>
-  </si>
-  <si>
-    <t>Effective and Management Communication</t>
-  </si>
-  <si>
-    <t>Negotiation and Selling Skills</t>
-  </si>
-  <si>
-    <t>Organisational Behaviour</t>
   </si>
   <si>
     <t>Course
@@ -362,6 +339,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -389,44 +399,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,7 +502,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2113"/>
+                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2115"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -28947,6 +28924,60 @@
           </cell>
           <cell r="BD135" t="str">
             <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Subjects List"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="C4" t="str">
+            <v>Perspective Management</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="C5" t="str">
+            <v>Financial Accounting</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="C6" t="str">
+            <v>Business Statistics</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7" t="str">
+            <v>Operations Management</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8" t="str">
+            <v>Managerial Economics</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="C9" t="str">
+            <v>Effective and Management Communication</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="C10" t="str">
+            <v>Negotiation and Selling Skills</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11" t="str">
+            <v>Organisational Behaviour</v>
           </cell>
         </row>
       </sheetData>
@@ -29277,104 +29308,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
     </row>
     <row r="6" spans="1:18" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -29392,223 +29423,223 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:18" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
     </row>
     <row r="8" spans="1:18" ht="9.9499999999999993" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="12"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="23"/>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
-        <v>26</v>
+      <c r="A9" s="9" t="s">
+        <v>18</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="27" t="str">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8" t="str">
         <f>VLOOKUP(D13,[1]Sheet1!$A:$B,2,0)</f>
         <v>ADEPU CHETAN GANESH ARCHANA</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="14"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="25"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>27</v>
+      <c r="A10" s="9" t="s">
+        <v>19</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="27" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="25"/>
+    </row>
+    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="25"/>
+    </row>
+    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="25"/>
+    </row>
+    <row r="13" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="14"/>
-    </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="14"/>
-    </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="14"/>
-    </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="16"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="27"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22" t="s">
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22" t="s">
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22" t="s">
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="18" t="s">
-        <v>18</v>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="15" t="s">
+        <v>10</v>
       </c>
-      <c r="O15" s="18" t="s">
-        <v>19</v>
+      <c r="O15" s="15" t="s">
+        <v>11</v>
       </c>
-      <c r="P15" s="18" t="s">
-        <v>20</v>
+      <c r="P15" s="15" t="s">
+        <v>12</v>
       </c>
-      <c r="Q15" s="18" t="s">
-        <v>21</v>
+      <c r="Q15" s="15" t="s">
+        <v>13</v>
       </c>
-      <c r="R15" s="18" t="s">
-        <v>22</v>
+      <c r="R15" s="15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="4" t="s">
         <v>5</v>
       </c>
@@ -29636,18 +29667,19 @@
       <c r="M16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="18"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>1</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>10</v>
+      <c r="B17" s="17" t="str">
+        <f>'[3]Subjects List'!$C4</f>
+        <v>Perspective Management</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -29704,8 +29736,9 @@
       <c r="A18" s="3">
         <v>2</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>11</v>
+      <c r="B18" s="17" t="str">
+        <f>'[3]Subjects List'!$C5</f>
+        <v>Financial Accounting</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -29762,8 +29795,9 @@
       <c r="A19" s="3">
         <v>3</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>12</v>
+      <c r="B19" s="17" t="str">
+        <f>'[3]Subjects List'!$C6</f>
+        <v>Business Statistics</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -29820,8 +29854,9 @@
       <c r="A20" s="3">
         <v>4</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>13</v>
+      <c r="B20" s="17" t="str">
+        <f>'[3]Subjects List'!$C7</f>
+        <v>Operations Management</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -29878,8 +29913,9 @@
       <c r="A21" s="3">
         <v>5</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>14</v>
+      <c r="B21" s="17" t="str">
+        <f>'[3]Subjects List'!$C8</f>
+        <v>Managerial Economics</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -29936,8 +29972,9 @@
       <c r="A22" s="3">
         <v>6</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>15</v>
+      <c r="B22" s="17" t="str">
+        <f>'[3]Subjects List'!$C9</f>
+        <v>Effective and Management Communication</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -29994,8 +30031,9 @@
       <c r="A23" s="3">
         <v>7</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>16</v>
+      <c r="B23" s="17" t="str">
+        <f>'[3]Subjects List'!$C10</f>
+        <v>Negotiation and Selling Skills</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -30052,8 +30090,9 @@
       <c r="A24" s="3">
         <v>8</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>17</v>
+      <c r="B24" s="17" t="str">
+        <f>'[3]Subjects List'!$C11</f>
+        <v>Organisational Behaviour</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -30107,18 +30146,18 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>23</v>
+      <c r="A25" s="11" t="s">
+        <v>15</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
       <c r="K25" s="3">
         <v>800</v>
       </c>
@@ -30139,104 +30178,104 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="str">
+      <c r="A26" s="12" t="str">
         <f>"Remarks : "&amp;VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BM$122,65,0)</f>
         <v>Remarks : Unsuccessful</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="24"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24" t="str">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12" t="str">
         <f>"SGPI : "&amp;VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BN$122,66,0)</f>
         <v>SGPI : 8.25</v>
       </c>
-      <c r="O26" s="24"/>
-      <c r="P26" s="23" t="str">
+      <c r="O26" s="12"/>
+      <c r="P26" s="13" t="str">
         <f>"Overall Grade:"&amp;VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BO$122,67,0)</f>
         <v>Overall Grade:A</v>
       </c>
-      <c r="Q26" s="23"/>
+      <c r="Q26" s="13"/>
       <c r="R26" s="6" t="str">
         <f>"Range:"&amp;VLOOKUP(D13,'[2]Subject Marks'!$A$3:$BP$122,68,0)</f>
         <v>Range:70.74.99</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
-        <v>24</v>
+      <c r="A27" s="12" t="s">
+        <v>16</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
     </row>
     <row r="28" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
-        <v>25</v>
+      <c r="A28" s="14" t="s">
+        <v>17</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="25"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P31" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="K32" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
@@ -30244,36 +30283,13 @@
       <c r="S32" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="nrblBHGUWzE+3MHaEBCJdBWws+2awurDuSo28c3l//Yk1yCV0gCkjLQVqzmBtyZ4lWKBYUrGx9a52Cg25uXkYQ==" saltValue="w4Aa6P7QvsaCwoVwwmCJ/g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="LcjzIpkW0YwBgD+jRaGekbdYBUyJz+ao7Z77uzi9jRAc6CGbnE5BcDZ4Ycc775t4l+WnQ3pWkMsCwZXESQJYHg==" saltValue="olPH5sTzzLtNTDw6Km7GYw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="D11" name="Held In"/>
     <protectedRange sqref="D13" name="Seat No."/>
     <protectedRange sqref="A27" name="Declared Date"/>
   </protectedRanges>
   <mergeCells count="39">
-    <mergeCell ref="D9:O9"/>
-    <mergeCell ref="D10:O10"/>
-    <mergeCell ref="D11:O11"/>
-    <mergeCell ref="D12:O12"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:O13"/>
-    <mergeCell ref="A25:J25"/>
-    <mergeCell ref="A26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="A27:R27"/>
-    <mergeCell ref="A28:R28"/>
-    <mergeCell ref="Q15:Q16"/>
-    <mergeCell ref="R15:R16"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="K15:M15"/>
     <mergeCell ref="A1:R5"/>
     <mergeCell ref="A7:R7"/>
     <mergeCell ref="A8:P8"/>
@@ -30290,6 +30306,29 @@
     <mergeCell ref="A14:M14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:D16"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="A27:R27"/>
+    <mergeCell ref="A28:R28"/>
+    <mergeCell ref="Q15:Q16"/>
+    <mergeCell ref="R15:R16"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:O13"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="D9:O9"/>
+    <mergeCell ref="D10:O10"/>
+    <mergeCell ref="D11:O11"/>
+    <mergeCell ref="D12:O12"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <pageMargins left="0.98425196850393704" right="0" top="0.78740157480314965" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Grade Card v3
Update Grade Card v3
</commit_message>
<xml_diff>
--- a/Batch 2018-20/Sem 1/Grade Card.xlsx
+++ b/Batch 2018-20/Sem 1/Grade Card.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Git\SIMSR-Results-Generator\Batch 2018-20\Sem 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFCDCDC-C087-4277-A20C-3F481D24D771}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56821EC3-6F65-4A4E-9D78-2CD803D23D97}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4C80AD8E-6BB5-43FA-A2DF-2A6A1A9D1C00}"/>
   </bookViews>
@@ -22,6 +22,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="PicUp">INDEX([1]Sheet1!$C$2:$C$121,MATCH('Final Grade Card'!$D$13:$I$13,[1]Sheet1!$A$2:$A$121,0))</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Final Grade Card'!$A$1:$I$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,9 +65,6 @@
     <t>Seal</t>
   </si>
   <si>
-    <t>Director</t>
-  </si>
-  <si>
     <t>MMS18-20/1</t>
   </si>
   <si>
@@ -96,9 +94,6 @@
     <t>Checked By  ______________</t>
   </si>
   <si>
-    <t>SIMSR</t>
-  </si>
-  <si>
     <t>PROGRAMME : MASTER OF MANAGEMENT STUDIES (SEMESTER -I)</t>
   </si>
   <si>
@@ -107,12 +102,19 @@
   <si>
     <t>PATTERN : CHOICE BASED CREDITS &amp; GRADING SYSTEM (CBCSGS)</t>
   </si>
+  <si>
+    <t>Sasmira's Institute of Mngmnt
+Studies and Research</t>
+  </si>
+  <si>
+    <t>Director / Controller of Examination</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +175,14 @@
     <font>
       <b/>
       <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -304,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -314,68 +324,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -394,6 +344,78 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,68 +436,18 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFDE4A27-FCA6-4BF6-999A-335F89A8FFDA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9526" y="9524"/>
-          <a:ext cx="5924550" cy="942975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>7</xdr:col>
-          <xdr:colOff>466725</xdr:colOff>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>28574</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>563822</xdr:colOff>
+          <xdr:colOff>954347</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>180974</xdr:rowOff>
         </xdr:to>
@@ -492,13 +464,13 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2127"/>
+                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2132"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
             <a:srcRect/>
             <a:stretch>
               <a:fillRect/>
@@ -506,8 +478,8 @@
           </xdr:blipFill>
           <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="4410075" y="1295399"/>
-              <a:ext cx="773372" cy="1038225"/>
+              <a:off x="4695825" y="1295399"/>
+              <a:ext cx="878147" cy="1038225"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -534,6 +506,50 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66751A2A-2BAB-4D1F-85FF-23C63FFAB6B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5743575" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -29354,15 +29370,15 @@
       <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
@@ -29378,141 +29394,141 @@
       <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="str">
+      <c r="A9" s="24" t="str">
         <f>"NAME OF THE CANDIDATE : "&amp;VLOOKUP(D13,[1]Sheet1!$A:$B,2,0)</f>
         <v>NAME OF THE CANDIDATE : ADEPU CHETAN GANESH ARCHANA</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-    </row>
-    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="19" t="s">
+      <c r="H15" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
     </row>
     <row r="17" spans="1:9" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>1</v>
       </c>
-      <c r="B17" s="18" t="str">
+      <c r="B17" s="19" t="str">
         <f>'[2]Subjects List'!$C$4</f>
         <v>Perspective Management</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="4">
         <v>4</v>
       </c>
@@ -29536,12 +29552,12 @@
       <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18" s="18" t="str">
+      <c r="B18" s="19" t="str">
         <f>'[2]Subjects List'!$C$5</f>
         <v>Financial Accounting</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="4">
         <v>4</v>
       </c>
@@ -29565,12 +29581,12 @@
       <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B19" s="18" t="str">
+      <c r="B19" s="19" t="str">
         <f>'[2]Subjects List'!$C$6</f>
         <v>Business Statistics</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="4">
         <v>4</v>
       </c>
@@ -29594,12 +29610,12 @@
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="18" t="str">
+      <c r="B20" s="19" t="str">
         <f>'[2]Subjects List'!$C$7</f>
         <v>Operations Management</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="4">
         <v>4</v>
       </c>
@@ -29623,12 +29639,12 @@
       <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21" s="18" t="str">
+      <c r="B21" s="19" t="str">
         <f>'[2]Subjects List'!$C$8</f>
         <v>Managerial Economics</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="4">
         <v>4</v>
       </c>
@@ -29652,12 +29668,12 @@
       <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B22" s="18" t="str">
+      <c r="B22" s="19" t="str">
         <f>'[2]Subjects List'!$C$9</f>
         <v>Effective and Management Communication</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="4">
         <v>4</v>
       </c>
@@ -29681,12 +29697,12 @@
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="18" t="str">
+      <c r="B23" s="19" t="str">
         <f>'[2]Subjects List'!$C$10</f>
         <v>Negotiation and Selling Skills</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="4">
         <v>4</v>
       </c>
@@ -29710,12 +29726,12 @@
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="18" t="str">
+      <c r="B24" s="19" t="str">
         <f>'[2]Subjects List'!$C$11</f>
         <v>Organisational Behaviour</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="4">
         <v>4</v>
       </c>
@@ -29737,50 +29753,53 @@
     </row>
     <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="23" t="s">
-        <v>10</v>
+      <c r="B25" s="28" t="s">
+        <v>9</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="25"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="5">
+      <c r="G25" s="32">
         <f>SUM(G17:G24)</f>
         <v>32</v>
       </c>
       <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="I25" s="31">
+        <f>SUM(I17:I24)</f>
+        <v>264</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="str">
+      <c r="A26" s="6" t="str">
         <f>"Remark    :  "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BM$122,65,0)</f>
         <v>Remark    :  Unsuccessful</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="29" t="str">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9" t="str">
         <f>"SGPI : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BN$122,66,0)</f>
         <v>SGPI : 8.25</v>
       </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="29" t="str">
+      <c r="F26" s="10"/>
+      <c r="G26" s="9" t="str">
         <f>"Overall Grade : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BO$122,67,0)</f>
         <v>Overall Grade : A</v>
       </c>
-      <c r="H26" s="30"/>
-      <c r="I26" s="6" t="str">
+      <c r="H26" s="10"/>
+      <c r="I26" s="5" t="str">
         <f>"Range : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BP$122,68,0)</f>
         <v>Range : 70-74.99</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
@@ -29813,7 +29832,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30"/>
       <c r="C30" s="2"/>
@@ -29831,11 +29850,11 @@
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31" s="8" t="s">
-        <v>8</v>
+      <c r="G31" s="35" t="s">
+        <v>21</v>
       </c>
-      <c r="I31" s="8"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32"/>
@@ -29843,27 +29862,26 @@
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
-      <c r="F32" t="s">
-        <v>7</v>
+      <c r="G32"/>
+      <c r="H32" s="33" t="s">
+        <v>20</v>
       </c>
-      <c r="G32"/>
-      <c r="H32" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="8"/>
+      <c r="I32" s="34"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
-      <c r="F33"/>
+      <c r="F33" t="s">
+        <v>7</v>
+      </c>
       <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34"/>
@@ -29877,17 +29895,17 @@
       <c r="I34"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -29896,11 +29914,22 @@
     <protectedRange sqref="A11" name="Held In"/>
   </protectedRanges>
   <mergeCells count="36">
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A1:I5"/>
+    <mergeCell ref="H32:I33"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="H8:I13"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="B15:D16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="C27:I27"/>
     <mergeCell ref="A7:I7"/>
@@ -29916,22 +29945,11 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A35:I35"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="H8:I13"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="B15:D16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A1:I5"/>
   </mergeCells>
   <pageMargins left="0.69" right="0" top="0.78740157480314965" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Grade Card to v3
Updated Grade Card to v3
</commit_message>
<xml_diff>
--- a/Batch 2018-20/Sem 1/Grade Card.xlsx
+++ b/Batch 2018-20/Sem 1/Grade Card.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Git\SIMSR-Results-Generator\Batch 2018-20\Sem 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56821EC3-6F65-4A4E-9D78-2CD803D23D97}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AEE7E8-168D-4D5A-8C8C-A498E2B63AE7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4C80AD8E-6BB5-43FA-A2DF-2A6A1A9D1C00}"/>
   </bookViews>
@@ -327,6 +327,75 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -347,75 +416,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,7 +464,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2132"/>
+                  <a14:cameraTool cellRange="PicUp" spid="_x0000_s2133"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -29315,220 +29315,220 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="A1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
     </row>
     <row r="6" spans="1:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:9" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
     </row>
     <row r="8" spans="1:9" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="str">
+      <c r="A9" s="12" t="str">
         <f>"NAME OF THE CANDIDATE : "&amp;VLOOKUP(D13,[1]Sheet1!$A:$B,2,0)</f>
         <v>NAME OF THE CANDIDATE : ADEPU CHETAN GANESH ARCHANA</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="24" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="20" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
     </row>
     <row r="17" spans="1:9" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>1</v>
       </c>
-      <c r="B17" s="19" t="str">
+      <c r="B17" s="18" t="str">
         <f>'[2]Subjects List'!$C$4</f>
         <v>Perspective Management</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="4">
         <v>4</v>
       </c>
@@ -29552,12 +29552,12 @@
       <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18" s="19" t="str">
+      <c r="B18" s="18" t="str">
         <f>'[2]Subjects List'!$C$5</f>
         <v>Financial Accounting</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="4">
         <v>4</v>
       </c>
@@ -29581,12 +29581,12 @@
       <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B19" s="19" t="str">
+      <c r="B19" s="18" t="str">
         <f>'[2]Subjects List'!$C$6</f>
         <v>Business Statistics</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="4">
         <v>4</v>
       </c>
@@ -29610,12 +29610,12 @@
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="19" t="str">
+      <c r="B20" s="18" t="str">
         <f>'[2]Subjects List'!$C$7</f>
         <v>Operations Management</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="4">
         <v>4</v>
       </c>
@@ -29639,12 +29639,12 @@
       <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21" s="19" t="str">
+      <c r="B21" s="18" t="str">
         <f>'[2]Subjects List'!$C$8</f>
         <v>Managerial Economics</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="4">
         <v>4</v>
       </c>
@@ -29668,12 +29668,12 @@
       <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B22" s="19" t="str">
+      <c r="B22" s="18" t="str">
         <f>'[2]Subjects List'!$C$9</f>
         <v>Effective and Management Communication</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="4">
         <v>4</v>
       </c>
@@ -29697,12 +29697,12 @@
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="19" t="str">
+      <c r="B23" s="18" t="str">
         <f>'[2]Subjects List'!$C$10</f>
         <v>Negotiation and Selling Skills</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="4">
         <v>4</v>
       </c>
@@ -29726,12 +29726,12 @@
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="19" t="str">
+      <c r="B24" s="18" t="str">
         <f>'[2]Subjects List'!$C$11</f>
         <v>Organisational Behaviour</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
       <c r="E24" s="4">
         <v>4</v>
       </c>
@@ -29753,60 +29753,60 @@
     </row>
     <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="30"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="32">
+      <c r="G25" s="7">
         <f>SUM(G17:G24)</f>
         <v>32</v>
       </c>
       <c r="H25" s="3"/>
-      <c r="I25" s="31">
+      <c r="I25" s="6">
         <f>SUM(I17:I24)</f>
         <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="str">
+      <c r="A26" s="29" t="str">
         <f>"Remark    :  "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BM$122,65,0)</f>
         <v>Remark    :  Unsuccessful</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="9" t="str">
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="32" t="str">
         <f>"SGPI : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BN$122,66,0)</f>
         <v>SGPI : 8.25</v>
       </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="9" t="str">
+      <c r="F26" s="33"/>
+      <c r="G26" s="32" t="str">
         <f>"Overall Grade : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BO$122,67,0)</f>
         <v>Overall Grade : A</v>
       </c>
-      <c r="H26" s="10"/>
+      <c r="H26" s="33"/>
       <c r="I26" s="5" t="str">
         <f>"Range : "&amp;VLOOKUP(D13,'[3]Subject Marks'!$A$3:$BP$122,68,0)</f>
         <v>Range : 70-74.99</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14" t="s">
+      <c r="B27" s="23"/>
+      <c r="C27" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="15"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="24"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28"/>
@@ -29850,11 +29850,11 @@
       <c r="D31"/>
       <c r="E31"/>
       <c r="F31"/>
-      <c r="G31" s="35" t="s">
+      <c r="G31" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32"/>
@@ -29863,10 +29863,10 @@
       <c r="D32"/>
       <c r="E32"/>
       <c r="G32"/>
-      <c r="H32" s="33" t="s">
+      <c r="H32" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I32" s="34"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -29880,8 +29880,8 @@
         <v>7</v>
       </c>
       <c r="G33"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34"/>
@@ -29895,25 +29895,46 @@
       <c r="I34"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="O6aSU7JLVSPOv7rHYM7zZDxE/BKz794fSGU4XnW6qsbUbTxzVLVdFQMc0wMmp+SmQfPJHP4jVsE70YKYR3SUpQ==" saltValue="62/2DfEFtOCkH3SmYLT2Dw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="C27" name="Declared Date"/>
     <protectedRange sqref="D13" name="Seat No."/>
     <protectedRange sqref="A11" name="Held In"/>
   </protectedRanges>
   <mergeCells count="36">
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A1:I5"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A26:D26"/>
     <mergeCell ref="H32:I33"/>
     <mergeCell ref="G31:I31"/>
     <mergeCell ref="A35:I35"/>
@@ -29930,26 +29951,6 @@
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B25:D25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A1:I5"/>
   </mergeCells>
   <pageMargins left="0.69" right="0" top="0.78740157480314965" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>